<commit_message>
#7 - Add buttsplice
</commit_message>
<xml_diff>
--- a/fdms/tests/sample_data.xlsx
+++ b/fdms/tests/sample_data.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BE" sheetId="1" r:id="rId1"/>
     <sheet name="BE_AMECO" sheetId="2" r:id="rId2"/>
     <sheet name="BE_ORIG" sheetId="3" r:id="rId3"/>
+    <sheet name="base_series1" sheetId="4" r:id="rId4"/>
+    <sheet name="test_splice1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="50">
   <si>
     <t>Country AMECO</t>
   </si>
@@ -507,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2299,10 +2301,13 @@
   <dimension ref="A1:BJ14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4801,4 +4806,507 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>1996</v>
+      </c>
+      <c r="I1">
+        <v>1997</v>
+      </c>
+      <c r="J1">
+        <v>1998</v>
+      </c>
+      <c r="K1">
+        <v>1999</v>
+      </c>
+      <c r="L1">
+        <v>2000</v>
+      </c>
+      <c r="M1">
+        <v>2001</v>
+      </c>
+      <c r="N1">
+        <v>2002</v>
+      </c>
+      <c r="O1">
+        <v>2003</v>
+      </c>
+      <c r="P1">
+        <v>2004</v>
+      </c>
+      <c r="Q1">
+        <v>2005</v>
+      </c>
+      <c r="R1">
+        <v>2006</v>
+      </c>
+      <c r="S1">
+        <v>2007</v>
+      </c>
+      <c r="T1">
+        <v>2008</v>
+      </c>
+      <c r="U1">
+        <v>2009</v>
+      </c>
+      <c r="V1">
+        <v>2010</v>
+      </c>
+      <c r="W1">
+        <v>2011</v>
+      </c>
+      <c r="X1">
+        <v>2012</v>
+      </c>
+      <c r="Y1">
+        <v>2013</v>
+      </c>
+      <c r="Z1">
+        <v>2014</v>
+      </c>
+      <c r="AA1">
+        <v>2015</v>
+      </c>
+      <c r="AB1">
+        <v>2016</v>
+      </c>
+      <c r="AC1">
+        <v>2017</v>
+      </c>
+      <c r="AD1">
+        <v>2018</v>
+      </c>
+      <c r="AE1">
+        <v>2019</v>
+      </c>
+      <c r="AF1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>714520000</v>
+      </c>
+      <c r="M2">
+        <v>808580000</v>
+      </c>
+      <c r="N2">
+        <v>918200000</v>
+      </c>
+      <c r="O2">
+        <v>999350000</v>
+      </c>
+      <c r="P2">
+        <v>1187470000</v>
+      </c>
+      <c r="Q2">
+        <v>1364510000</v>
+      </c>
+      <c r="R2">
+        <v>1726780000</v>
+      </c>
+      <c r="S2">
+        <v>2072000000</v>
+      </c>
+      <c r="T2">
+        <v>1894140000</v>
+      </c>
+      <c r="U2">
+        <v>1965010000</v>
+      </c>
+      <c r="V2">
+        <v>1934920000</v>
+      </c>
+      <c r="W2">
+        <v>2150610000</v>
+      </c>
+      <c r="X2">
+        <v>2366150000</v>
+      </c>
+      <c r="Y2">
+        <v>2417210000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BQ2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BL1" sqref="BL1:BQ1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="38" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>1960</v>
+      </c>
+      <c r="E1">
+        <v>1961</v>
+      </c>
+      <c r="F1">
+        <v>1962</v>
+      </c>
+      <c r="G1">
+        <v>1963</v>
+      </c>
+      <c r="H1">
+        <v>1964</v>
+      </c>
+      <c r="I1">
+        <v>1965</v>
+      </c>
+      <c r="J1">
+        <v>1966</v>
+      </c>
+      <c r="K1">
+        <v>1967</v>
+      </c>
+      <c r="L1">
+        <v>1968</v>
+      </c>
+      <c r="M1">
+        <v>1969</v>
+      </c>
+      <c r="N1">
+        <v>1970</v>
+      </c>
+      <c r="O1">
+        <v>1971</v>
+      </c>
+      <c r="P1">
+        <v>1972</v>
+      </c>
+      <c r="Q1">
+        <v>1973</v>
+      </c>
+      <c r="R1">
+        <v>1974</v>
+      </c>
+      <c r="S1">
+        <v>1975</v>
+      </c>
+      <c r="T1">
+        <v>1976</v>
+      </c>
+      <c r="U1">
+        <v>1977</v>
+      </c>
+      <c r="V1">
+        <v>1978</v>
+      </c>
+      <c r="W1">
+        <v>1979</v>
+      </c>
+      <c r="X1">
+        <v>1980</v>
+      </c>
+      <c r="Y1">
+        <v>1981</v>
+      </c>
+      <c r="Z1">
+        <v>1982</v>
+      </c>
+      <c r="AA1">
+        <v>1983</v>
+      </c>
+      <c r="AB1">
+        <v>1984</v>
+      </c>
+      <c r="AC1">
+        <v>1985</v>
+      </c>
+      <c r="AD1">
+        <v>1986</v>
+      </c>
+      <c r="AE1">
+        <v>1987</v>
+      </c>
+      <c r="AF1">
+        <v>1988</v>
+      </c>
+      <c r="AG1">
+        <v>1989</v>
+      </c>
+      <c r="AH1">
+        <v>1990</v>
+      </c>
+      <c r="AI1">
+        <v>1991</v>
+      </c>
+      <c r="AJ1">
+        <v>1992</v>
+      </c>
+      <c r="AK1">
+        <v>1993</v>
+      </c>
+      <c r="AL1">
+        <v>1994</v>
+      </c>
+      <c r="AM1">
+        <v>1995</v>
+      </c>
+      <c r="AN1">
+        <v>1996</v>
+      </c>
+      <c r="AO1">
+        <v>1997</v>
+      </c>
+      <c r="AP1">
+        <v>1998</v>
+      </c>
+      <c r="AQ1">
+        <v>1999</v>
+      </c>
+      <c r="AR1">
+        <v>2000</v>
+      </c>
+      <c r="AS1">
+        <v>2001</v>
+      </c>
+      <c r="AT1">
+        <v>2002</v>
+      </c>
+      <c r="AU1">
+        <v>2003</v>
+      </c>
+      <c r="AV1">
+        <v>2004</v>
+      </c>
+      <c r="AW1">
+        <v>2005</v>
+      </c>
+      <c r="AX1">
+        <v>2006</v>
+      </c>
+      <c r="AY1">
+        <v>2007</v>
+      </c>
+      <c r="AZ1">
+        <v>2008</v>
+      </c>
+      <c r="BA1">
+        <v>2009</v>
+      </c>
+      <c r="BB1">
+        <v>2010</v>
+      </c>
+      <c r="BC1">
+        <v>2011</v>
+      </c>
+      <c r="BD1">
+        <v>2012</v>
+      </c>
+      <c r="BE1">
+        <v>2013</v>
+      </c>
+      <c r="BF1">
+        <v>2014</v>
+      </c>
+      <c r="BG1">
+        <v>2015</v>
+      </c>
+      <c r="BH1">
+        <v>2016</v>
+      </c>
+      <c r="BI1">
+        <v>2017</v>
+      </c>
+      <c r="BJ1">
+        <v>2018</v>
+      </c>
+      <c r="BK1">
+        <v>2019</v>
+      </c>
+      <c r="BL1">
+        <v>2020</v>
+      </c>
+      <c r="BM1">
+        <v>2021</v>
+      </c>
+      <c r="BN1">
+        <v>2022</v>
+      </c>
+      <c r="BO1">
+        <v>2023</v>
+      </c>
+      <c r="BP1">
+        <v>2024</v>
+      </c>
+      <c r="BQ1">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM2">
+        <v>22.745999999999999</v>
+      </c>
+      <c r="AN2">
+        <v>23.991</v>
+      </c>
+      <c r="AO2">
+        <v>25.373999999999999</v>
+      </c>
+      <c r="AP2">
+        <v>26.329000000000001</v>
+      </c>
+      <c r="AQ2">
+        <v>28.177</v>
+      </c>
+      <c r="AR2">
+        <v>29.687000000000001</v>
+      </c>
+      <c r="AS2">
+        <v>29.276</v>
+      </c>
+      <c r="AT2">
+        <v>30.504999999999999</v>
+      </c>
+      <c r="AU2">
+        <v>31.297999999999998</v>
+      </c>
+      <c r="AV2">
+        <v>33.625</v>
+      </c>
+      <c r="AW2">
+        <v>35.67</v>
+      </c>
+      <c r="AX2">
+        <v>37.241</v>
+      </c>
+      <c r="AY2">
+        <v>39.244</v>
+      </c>
+      <c r="AZ2">
+        <v>39.414000000000001</v>
+      </c>
+      <c r="BA2">
+        <v>38.091999999999999</v>
+      </c>
+      <c r="BB2">
+        <v>40.911999999999999</v>
+      </c>
+      <c r="BC2">
+        <v>41.972000000000001</v>
+      </c>
+      <c r="BD2">
+        <v>42.976999999999997</v>
+      </c>
+      <c r="BE2">
+        <v>43.548000000000002</v>
+      </c>
+      <c r="BF2">
+        <v>44.174999999999997</v>
+      </c>
+      <c r="BG2">
+        <v>45.094000000000001</v>
+      </c>
+      <c r="BH2">
+        <v>47.523897959999999</v>
+      </c>
+      <c r="BI2">
+        <v>49.801243100000001</v>
+      </c>
+      <c r="BJ2">
+        <v>51.711805529999999</v>
+      </c>
+      <c r="BK2">
+        <v>54.065427079999999</v>
+      </c>
+      <c r="BL2">
+        <v>56.278503252999997</v>
+      </c>
+      <c r="BM2">
+        <v>58.491579426000001</v>
+      </c>
+      <c r="BN2">
+        <v>60.704655598999999</v>
+      </c>
+      <c r="BO2">
+        <v>62.917731772000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#7 - Add more tests
</commit_message>
<xml_diff>
--- a/fdms/tests/sample_data.xlsx
+++ b/fdms/tests/sample_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BE" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="BE_ORIG" sheetId="3" r:id="rId3"/>
     <sheet name="base_series1" sheetId="4" r:id="rId4"/>
     <sheet name="test_splice1" sheetId="5" r:id="rId5"/>
+    <sheet name="quarterly_series" sheetId="6" r:id="rId6"/>
+    <sheet name="empty_series" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="76">
   <si>
     <t>Country AMECO</t>
   </si>
@@ -168,6 +170,84 @@
   </si>
   <si>
     <t>UTVTBP_blanks</t>
+  </si>
+  <si>
+    <t>2000Q1</t>
+  </si>
+  <si>
+    <t>2000Q2</t>
+  </si>
+  <si>
+    <t>2000Q3</t>
+  </si>
+  <si>
+    <t>2000Q4</t>
+  </si>
+  <si>
+    <t>2001Q1</t>
+  </si>
+  <si>
+    <t>2001Q2</t>
+  </si>
+  <si>
+    <t>2001Q3</t>
+  </si>
+  <si>
+    <t>2001Q4</t>
+  </si>
+  <si>
+    <t>2002Q1</t>
+  </si>
+  <si>
+    <t>2002Q2</t>
+  </si>
+  <si>
+    <t>2002Q3</t>
+  </si>
+  <si>
+    <t>2002Q4</t>
+  </si>
+  <si>
+    <t>2003Q4</t>
+  </si>
+  <si>
+    <t>2003Q1</t>
+  </si>
+  <si>
+    <t>2003Q2</t>
+  </si>
+  <si>
+    <t>2003Q3</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>indexes</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>YYYYQX</t>
+  </si>
+  <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>is</t>
   </si>
 </sst>
 </file>
@@ -4813,7 +4893,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4938,12 +5018,6 @@
       <c r="L2">
         <v>714520000</v>
       </c>
-      <c r="M2">
-        <v>808580000</v>
-      </c>
-      <c r="N2">
-        <v>918200000</v>
-      </c>
       <c r="O2">
         <v>999350000</v>
       </c>
@@ -4980,6 +5054,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4987,8 +5062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BL1" sqref="BL1:BQ1"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2:BO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5308,5 +5383,245 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>22.745999999999999</v>
+      </c>
+      <c r="E2">
+        <v>23.991</v>
+      </c>
+      <c r="F2">
+        <v>25.373999999999999</v>
+      </c>
+      <c r="G2">
+        <v>26.329000000000001</v>
+      </c>
+      <c r="H2">
+        <v>28.177</v>
+      </c>
+      <c r="I2">
+        <v>29.687000000000001</v>
+      </c>
+      <c r="J2">
+        <v>29.276</v>
+      </c>
+      <c r="K2">
+        <v>30.504999999999999</v>
+      </c>
+      <c r="L2">
+        <v>31.297999999999998</v>
+      </c>
+      <c r="M2">
+        <v>33.625</v>
+      </c>
+      <c r="N2">
+        <v>35.67</v>
+      </c>
+      <c r="O2">
+        <v>37.241</v>
+      </c>
+      <c r="P2">
+        <v>39.244</v>
+      </c>
+      <c r="Q2">
+        <v>39.414000000000001</v>
+      </c>
+      <c r="R2">
+        <v>38.091999999999999</v>
+      </c>
+      <c r="S2">
+        <v>40.911999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>22.745999999999999</v>
+      </c>
+      <c r="E2">
+        <v>23.991</v>
+      </c>
+      <c r="F2">
+        <v>25.373999999999999</v>
+      </c>
+      <c r="G2">
+        <v>26.329000000000001</v>
+      </c>
+      <c r="H2">
+        <v>28.177</v>
+      </c>
+      <c r="I2">
+        <v>29.687000000000001</v>
+      </c>
+      <c r="J2">
+        <v>29.276</v>
+      </c>
+      <c r="K2">
+        <v>30.504999999999999</v>
+      </c>
+      <c r="L2">
+        <v>31.297999999999998</v>
+      </c>
+      <c r="M2">
+        <v>33.625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>